<commit_message>
update emission cap for india and row based on new changes
</commit_message>
<xml_diff>
--- a/input/India_NDC/NZ_India+ROW trajectory.xlsx
+++ b/input/India_NDC/NZ_India+ROW trajectory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RPS+NZ" sheetId="1" r:id="rId1"/>
@@ -1388,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1644,7 +1644,7 @@
         <v>5883.3893388522702</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" ref="D10:K10" si="1">D8-D3</f>
+        <f t="shared" ref="D10:J10" si="1">D8-D3</f>
         <v>7709.5535523787903</v>
       </c>
       <c r="E10" s="4">
@@ -1671,43 +1671,43 @@
         <f t="shared" si="1"/>
         <v>11024.96760155121</v>
       </c>
-      <c r="K10" s="4">
-        <v>10761.130045503751</v>
+      <c r="K10">
+        <v>10762.418982612529</v>
       </c>
       <c r="L10" s="4">
         <v>0.01</v>
       </c>
       <c r="M10" s="4">
         <f>TREND($K$10:$L$10,$K$7:$L$7,M7)</f>
-        <v>9415.990039815777</v>
+        <v>9417.1178597859107</v>
       </c>
       <c r="N10" s="4">
         <f t="shared" ref="N10:T10" si="2">TREND($K$10:$L$10,$K$7:$L$7,N7)</f>
-        <v>8070.8500341278268</v>
+        <v>8071.8167369592702</v>
       </c>
       <c r="O10" s="4">
         <f t="shared" si="2"/>
-        <v>6725.7100284398766</v>
+        <v>6726.5156141327461</v>
       </c>
       <c r="P10" s="4">
         <f t="shared" si="2"/>
-        <v>5380.5700227519264</v>
+        <v>5381.214491306222</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>4035.4300170639763</v>
+        <v>4035.9133684795815</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="2"/>
-        <v>2690.2900113760261</v>
+        <v>2690.6122456530575</v>
       </c>
       <c r="S10" s="4">
         <f t="shared" si="2"/>
-        <v>1345.1500056879595</v>
+        <v>1345.311122826417</v>
       </c>
       <c r="T10" s="4">
         <f t="shared" si="2"/>
-        <v>1.0000000009313226E-2</v>
+        <v>9.9999998928979039E-3</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
@@ -1788,54 +1788,54 @@
         <v>5</v>
       </c>
       <c r="C15">
-        <v>162.91283410715999</v>
+        <v>158.96183844116999</v>
       </c>
       <c r="D15">
-        <v>336.15795273330002</v>
+        <v>330.14207993359997</v>
       </c>
       <c r="E15">
-        <v>493.33151433099999</v>
+        <v>486.09461641299998</v>
       </c>
       <c r="F15">
-        <v>625.17296249999902</v>
+        <v>614.821160649999</v>
       </c>
       <c r="G15">
-        <v>707.67303663637995</v>
+        <v>692.55422120976698</v>
       </c>
       <c r="H15">
-        <v>847.19036785036997</v>
+        <v>815.97183316859002</v>
       </c>
       <c r="I15">
-        <v>1007.17804229071</v>
+        <v>952.64733088577998</v>
       </c>
       <c r="J15">
-        <v>1171.5752754396301</v>
+        <v>1098.9321855661301</v>
       </c>
       <c r="K15">
-        <v>1257.4234165395501</v>
+        <v>1252.3569714544701</v>
       </c>
       <c r="L15" s="4">
         <v>0.01</v>
       </c>
       <c r="M15">
         <f>TREND($K$15:$L$15,$K$14:$L$14,M14)</f>
-        <v>1047.8545137829497</v>
+        <v>1043.6324762120639</v>
       </c>
       <c r="N15">
         <f t="shared" ref="N15:Q15" si="3">TREND($K$15:$L$15,$K$14:$L$14,N14)</f>
-        <v>838.28561102636741</v>
+        <v>834.90798096964136</v>
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
-        <v>628.71670826977061</v>
+        <v>626.18348572723335</v>
       </c>
       <c r="P15">
         <f t="shared" si="3"/>
-        <v>419.14780551317381</v>
+        <v>417.45899048482534</v>
       </c>
       <c r="Q15">
         <f t="shared" si="3"/>
-        <v>209.57890275659156</v>
+        <v>208.73449524241732</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1850,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
-      <selection activeCell="P31" sqref="A29:P31"/>
+    <sheetView topLeftCell="E12" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2331,54 +2331,54 @@
         <v>9051.5947628630693</v>
       </c>
       <c r="F17">
-        <v>9611.89411076959</v>
+        <v>9611.8941087795902</v>
       </c>
       <c r="G17">
-        <v>10380.3089735103</v>
+        <v>10388.3306887572</v>
       </c>
       <c r="H17">
-        <v>10928.885569481799</v>
+        <v>10935.9306832204</v>
       </c>
       <c r="I17">
-        <v>11408.584842424199</v>
+        <v>11408.795607062901</v>
       </c>
       <c r="J17">
-        <v>11731.8642222156</v>
+        <v>11730.2085455776</v>
       </c>
       <c r="K17">
-        <v>12018.553462043301</v>
+        <v>12014.775954066999</v>
       </c>
       <c r="L17" s="5">
         <f>L18+L22</f>
-        <v>10422.538699446333</v>
+        <v>10423.666519416467</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" ref="M17:S17" si="0">M18+M22</f>
-        <v>8876.0909618322767</v>
+        <v>8877.0576646637201</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="0"/>
-        <v>7329.6432242182054</v>
+        <v>7330.4488099110749</v>
       </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>5783.1954866041488</v>
+        <v>5783.8399551584444</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="0"/>
-        <v>4236.7477489900921</v>
+        <v>4237.2311004056974</v>
       </c>
       <c r="Q17" s="5">
         <f t="shared" si="0"/>
-        <v>2690.3000113760208</v>
+        <v>2690.6222456530522</v>
       </c>
       <c r="R17" s="5">
         <f t="shared" si="0"/>
-        <v>1345.1500056879595</v>
+        <v>1345.311122826417</v>
       </c>
       <c r="S17" s="5">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>9.9999998928979039E-3</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
@@ -2399,51 +2399,51 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>8997.073082219591</v>
+        <v>8997.0729481295912</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>9695.7171694685476</v>
+        <v>9695.7764675474336</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>10119.871321536782</v>
+        <v>10119.958850051809</v>
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>10454.85197341863</v>
+        <v>10456.14827617712</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>10629.607607217829</v>
+        <v>10631.27636001147</v>
       </c>
       <c r="K18">
         <f t="shared" si="1"/>
-        <v>10761.130045503751</v>
+        <v>10762.418982612529</v>
       </c>
       <c r="L18" s="9">
-        <v>9415.990039815777</v>
+        <v>9417.1178597859107</v>
       </c>
       <c r="M18" s="9">
-        <v>8070.8500341278268</v>
+        <v>8071.8167369592702</v>
       </c>
       <c r="N18" s="9">
-        <v>6725.7100284398766</v>
+        <v>6726.5156141327461</v>
       </c>
       <c r="O18" s="9">
-        <v>5380.5700227519264</v>
+        <v>5381.214491306222</v>
       </c>
       <c r="P18" s="9">
-        <v>4035.4300170639763</v>
+        <v>4035.9133684795815</v>
       </c>
       <c r="Q18" s="9">
-        <v>2690.2900113760261</v>
+        <v>2690.6122456530575</v>
       </c>
       <c r="R18" s="9">
-        <v>1345.1500056879595</v>
+        <v>1345.311122826417</v>
       </c>
       <c r="S18" s="1">
-        <v>0.01</v>
+        <v>9.9999998928979039E-3</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.35">
@@ -2655,40 +2655,40 @@
         <v>486.09461641299998</v>
       </c>
       <c r="F26">
-        <v>614.82102854999903</v>
+        <v>614.821160649999</v>
       </c>
       <c r="G26">
-        <v>684.59180404175299</v>
+        <v>692.55422120976698</v>
       </c>
       <c r="H26">
-        <v>809.01424794501702</v>
+        <v>815.97183316859002</v>
       </c>
       <c r="I26">
-        <v>953.73286900557002</v>
+        <v>952.64733088577998</v>
       </c>
       <c r="J26">
-        <v>1102.2566149977699</v>
+        <v>1098.9321855661301</v>
       </c>
       <c r="K26">
-        <v>1257.4234165395501</v>
+        <v>1252.3569714544701</v>
       </c>
       <c r="L26" s="9">
-        <v>1047.8545137829497</v>
+        <v>1043.6324762120639</v>
       </c>
       <c r="M26" s="9">
-        <v>838.28561102636741</v>
+        <v>834.90798096964136</v>
       </c>
       <c r="N26" s="9">
-        <v>628.71670826977061</v>
+        <v>626.18348572723335</v>
       </c>
       <c r="O26" s="9">
-        <v>419.14780551317381</v>
+        <v>417.45899048482534</v>
       </c>
       <c r="P26" s="9">
-        <v>209.57890275659156</v>
+        <v>208.73449524241732</v>
       </c>
       <c r="Q26" s="9">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="R26">
         <v>0</v>

</xml_diff>